<commit_message>
wip(writing): started writing in evaluataion
</commit_message>
<xml_diff>
--- a/evaluation/usecase 1/results.xlsx
+++ b/evaluation/usecase 1/results.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18217"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27610"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89EB7571-2359-4447-B001-3A6215608B91}" xr6:coauthVersionLast="19" xr6:coauthVersionMax="19" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aly/Master-Thesis/evaluation/usecase 1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Tensor</t>
   </si>
@@ -54,16 +66,19 @@
   </si>
   <si>
     <t>tensor</t>
+  </si>
+  <si>
+    <t>STDEV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,21 +425,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="4" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="4" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -438,7 +453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -452,7 +467,7 @@
         <v>20.826000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -466,7 +481,7 @@
         <v>19.050999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -480,7 +495,7 @@
         <v>29.425000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -494,7 +509,7 @@
         <v>32.68</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -508,7 +523,7 @@
         <v>22.626999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -522,7 +537,7 @@
         <v>15.922000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -536,7 +551,7 @@
         <v>43.311</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -550,7 +565,7 @@
         <v>28.626999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -567,528 +582,580 @@
         <v>26.558625000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3">
+        <f>STDEV(B2:B9)</f>
+        <v>1.4395315706357885</v>
+      </c>
+      <c r="C11" s="3">
+        <f>STDEV(C2:C9)</f>
+        <v>8.8299316774577274</v>
+      </c>
+      <c r="D11" s="3">
+        <f>STDEV(D2:D9)</f>
+        <v>8.8513959340966526</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>1</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B15" s="3">
         <v>0.104</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C15" s="3">
         <v>2.3860000000000001</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D15" s="3">
         <v>2.2330000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <v>2</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="3">
         <v>0.106</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C16" s="3">
         <v>2.323</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D16" s="3">
         <v>2.3479999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>3</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B17" s="3">
         <v>0.09</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C17" s="3">
         <v>2.3210000000000002</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D17" s="3">
         <v>1.38</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
         <v>4</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B18" s="3">
         <v>0.08</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C18" s="3">
         <v>2.34</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D18" s="3">
         <v>1.2749999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>5</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B19" s="3">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C19" s="3">
         <v>2.21</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D19" s="3">
         <v>1.4410000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>6</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B20" s="3">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C20" s="3">
         <v>2.2989999999999999</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D20" s="3">
         <v>2.2469999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>7</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B21" s="3">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C21" s="3">
         <v>2.3290000000000002</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D21" s="3">
         <v>2.2109999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
         <v>8</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B22" s="3">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C22" s="3">
         <v>2.3679999999999999</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D22" s="3">
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="3" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="3">
-        <f>AVERAGE(B14:B21)</f>
+      <c r="B23" s="3">
+        <f>AVERAGE(B15:B22)</f>
         <v>8.7374999999999994E-2</v>
       </c>
-      <c r="C22" s="3">
-        <f>AVERAGE(C14:C21)</f>
+      <c r="C23" s="3">
+        <f>AVERAGE(C15:C22)</f>
         <v>2.3219999999999996</v>
       </c>
-      <c r="D22" s="3">
-        <f>AVERAGE(D14:D21)</f>
+      <c r="D23" s="3">
+        <f>AVERAGE(D15:D22)</f>
         <v>1.9481250000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="3">
+        <f>STDEV(B15:B22)</f>
+        <v>1.2153041947242265E-2</v>
+      </c>
+      <c r="C24" s="3">
+        <f>STDEV(C15:C22)</f>
+        <v>5.2995956719087828E-2</v>
+      </c>
+      <c r="D24" s="3">
+        <f>STDEV(D15:D22)</f>
+        <v>0.49053918949312414</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
         <v>1</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B29" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C29" s="3">
         <v>0.76100000000000001</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D29" s="3">
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
         <v>2</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B30" s="3">
         <v>0.16300000000000001</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C30" s="3">
         <v>0.79900000000000004</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D30" s="3">
         <v>0.79900000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
         <v>3</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B31" s="3">
         <v>0.125</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C31" s="3">
         <v>0.92700000000000005</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D31" s="3">
         <v>0.92300000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
         <v>4</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B32" s="3">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C32" s="3">
         <v>0.752</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D32" s="3">
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="4">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
         <v>5</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B33" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C33" s="3">
         <v>0.81399999999999995</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D33" s="3">
         <v>0.77800000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="4">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
         <v>6</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B34" s="3">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C34" s="3">
         <v>0.82399999999999995</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D34" s="3">
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="4">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
         <v>7</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B35" s="3">
         <v>9.4E-2</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C35" s="3">
         <v>0.73599999999999999</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D35" s="3">
         <v>0.83499999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="4">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
         <v>8</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B36" s="3">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C36" s="3">
         <v>0.79800000000000004</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D36" s="3">
         <v>0.76900000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="3" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="3">
-        <f>AVERAGE(B27:B34)</f>
+      <c r="B37" s="3">
+        <f>AVERAGE(B29:B36)</f>
         <v>0.10474999999999998</v>
       </c>
-      <c r="C35" s="3">
-        <f>AVERAGE(C27:C34)</f>
+      <c r="C37" s="3">
+        <f>AVERAGE(C29:C36)</f>
         <v>0.80137499999999995</v>
       </c>
-      <c r="D35" s="3">
-        <f>AVERAGE(D27:D34)</f>
+      <c r="D37" s="3">
+        <f>AVERAGE(D29:D36)</f>
         <v>0.83387499999999992</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="3" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="3">
+        <f>STDEV(B29:B36)</f>
+        <v>2.7937430089398082E-2</v>
+      </c>
+      <c r="C38" s="3">
+        <f>STDEV(C29:C36)</f>
+        <v>5.9536153481969029E-2</v>
+      </c>
+      <c r="D38" s="3">
+        <f>STDEV(D29:D36)</f>
+        <v>5.128195867665631E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E42" t="s">
         <v>11</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F42" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="1">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
         <v>1</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B43" s="1">
         <v>0.26600000000000001</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C43" s="1">
         <v>0.65900000000000003</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D43" s="1">
         <v>0.27600000000000002</v>
       </c>
-      <c r="E40">
+      <c r="E43">
         <v>0.68600000000000005</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F43" s="3">
         <v>5.5819999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="1">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
         <v>2</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B44" s="1">
         <v>0.29599999999999999</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C44" s="1">
         <v>0.67400000000000004</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D44" s="1">
         <v>0.32300000000000001</v>
       </c>
-      <c r="E41">
+      <c r="E44">
         <v>0.79</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F44" s="3">
         <v>5.6395</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="1">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
         <v>3</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B45" s="1">
         <v>0.186</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C45" s="1">
         <v>0.72799999999999998</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D45" s="1">
         <v>0.313</v>
       </c>
-      <c r="E42">
+      <c r="E45">
         <v>0.67600000000000005</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F45" s="3">
         <v>5.5730000000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="1">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
         <v>4</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B46" s="1">
         <v>0.34200000000000003</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C46" s="1">
         <v>0.80700000000000005</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D46" s="1">
         <v>0.222</v>
       </c>
-      <c r="E43">
+      <c r="E46">
         <v>0.66100000000000003</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F46" s="3">
         <v>4.9400000000000004</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="1">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>5</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B47" s="1">
         <v>0.22700000000000001</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C47" s="1">
         <v>0.752</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D47" s="1">
         <v>0.219</v>
       </c>
-      <c r="E44">
+      <c r="E47">
         <v>0.72199999999999998</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F47" s="3">
         <v>5.6029999999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="1">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>6</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B48" s="1">
         <v>0.26200000000000001</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C48" s="1">
         <v>0.71299999999999997</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D48" s="1">
         <v>0.32200000000000001</v>
       </c>
-      <c r="E45">
+      <c r="E48">
         <v>0.74199999999999999</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F48" s="3">
         <v>5.5990000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="1">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
         <v>7</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B49" s="1">
         <v>0.30599999999999999</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C49" s="1">
         <v>0.68400000000000005</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D49" s="1">
         <v>0.21199999999999999</v>
       </c>
-      <c r="E46">
+      <c r="E49">
         <v>0.66300000000000003</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F49" s="3">
         <v>5.5750000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="1">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>8</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B50" s="1">
         <v>0.374</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C50" s="1">
         <v>0.58199999999999996</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D50" s="1">
         <v>0.29299999999999998</v>
       </c>
-      <c r="E47">
+      <c r="E50">
         <v>0.64800000000000002</v>
       </c>
-      <c r="F47">
+      <c r="F50">
         <v>5.5810000000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="3" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="3">
-        <f>AVERAGE(B40:B47)</f>
+      <c r="B51" s="3">
+        <f>AVERAGE(B43:B50)</f>
         <v>0.28237500000000004</v>
       </c>
-      <c r="C48" s="3">
-        <f>AVERAGE(C40:C47)</f>
+      <c r="C51" s="3">
+        <f>AVERAGE(C43:C50)</f>
         <v>0.69987500000000002</v>
       </c>
-      <c r="D48" s="3">
-        <f>AVERAGE(D40:D47)</f>
+      <c r="D51" s="3">
+        <f>AVERAGE(D43:D50)</f>
         <v>0.27250000000000002</v>
       </c>
-      <c r="E48">
-        <f>AVERAGE(E40:E47)</f>
+      <c r="E51">
+        <f>AVERAGE(E43:E50)</f>
         <v>0.69850000000000001</v>
       </c>
-      <c r="F48" s="5">
-        <f>AVERAGE(F40:F47)</f>
+      <c r="F51" s="5">
+        <f>AVERAGE(F43:F50)</f>
         <v>5.5115625000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add(writing): added text to the evaluation
</commit_message>
<xml_diff>
--- a/evaluation/usecase 1/results.xlsx
+++ b/evaluation/usecase 1/results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Tensor</t>
   </si>
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -121,7 +121,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F52" sqref="A51:F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1125,7 +1124,7 @@
       <c r="E50">
         <v>0.64800000000000002</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="1">
         <v>5.5810000000000004</v>
       </c>
     </row>
@@ -1149,9 +1148,34 @@
         <f>AVERAGE(E43:E50)</f>
         <v>0.69850000000000001</v>
       </c>
-      <c r="F51" s="5">
+      <c r="F51" s="3">
         <f>AVERAGE(F43:F50)</f>
         <v>5.5115625000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="3">
+        <f>STDEV(B43:B50)</f>
+        <v>6.062987830151996E-2</v>
+      </c>
+      <c r="C52" s="3">
+        <f>STDEV(C43:C50)</f>
+        <v>6.7233999689782817E-2</v>
+      </c>
+      <c r="D52" s="3">
+        <f>STDEV(D43:D50)</f>
+        <v>4.8026778244760621E-2</v>
+      </c>
+      <c r="E52">
+        <f>STDEV(E43:E50)</f>
+        <v>4.8837924373818925E-2</v>
+      </c>
+      <c r="F52" s="3">
+        <f>STDEV(F43:F51)</f>
+        <v>0.21697918066890645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>